<commit_message>
新加直接 属性:数值   属性:数值% 填表方式 	修改：     .vscode/launch.json 	修改：     v2/example/AAA.xlsx 	修改：     v2/example/Globals.xlsx 	修改：     v2/filter/structparser.go 	修改：     v2/sheet_data.go
</commit_message>
<xml_diff>
--- a/v2/example/AAA.xlsx
+++ b/v2/example/AAA.xlsx
@@ -1,32 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10512"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luozhenya/gopath/src/github.com/adamluo159/tabtoy/v2/example/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{689C2D15-EBE8-B742-908B-7595E89EF4A7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-35140" yWindow="5280" windowWidth="28800" windowHeight="13460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowWidth="28060" windowHeight="13460"/>
   </bookViews>
   <sheets>
     <sheet name="AAA" sheetId="1" r:id="rId1"/>
     <sheet name="@Types" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="144525" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Administrator</author>
   </authors>
   <commentList>
-    <comment ref="A3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="A3" authorId="0">
       <text>
         <r>
           <rPr>
@@ -34,7 +28,6 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="宋体"/>
-            <family val="3"/>
             <charset val="134"/>
           </rPr>
           <t>Administrator:</t>
@@ -44,7 +37,6 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="宋体"/>
-            <family val="3"/>
             <charset val="134"/>
           </rPr>
           <t xml:space="preserve">
@@ -57,20 +49,19 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Administrator</author>
     <author>Davy</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
+    <comment ref="A1" authorId="0">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="9"/>
             <rFont val="宋体"/>
-            <family val="3"/>
             <charset val="134"/>
           </rPr>
           <t>Administrator:</t>
@@ -79,7 +70,6 @@
           <rPr>
             <sz val="9"/>
             <rFont val="宋体"/>
-            <family val="3"/>
             <charset val="134"/>
           </rPr>
           <t xml:space="preserve">
@@ -87,7 +77,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
+    <comment ref="D2" authorId="0">
       <text>
         <r>
           <rPr>
@@ -95,7 +85,6 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="宋体"/>
-            <family val="3"/>
             <charset val="134"/>
           </rPr>
           <t>Administrator:</t>
@@ -105,7 +94,6 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="宋体"/>
-            <family val="3"/>
             <charset val="134"/>
           </rPr>
           <t xml:space="preserve">
@@ -113,7 +101,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E2" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0100-000003000000}">
+    <comment ref="E2" authorId="1">
       <text>
         <r>
           <rPr>
@@ -121,7 +109,6 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="宋体"/>
-            <family val="3"/>
             <charset val="134"/>
           </rPr>
           <t>Davy:</t>
@@ -131,7 +118,6 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="宋体"/>
-            <family val="3"/>
             <charset val="134"/>
           </rPr>
           <t xml:space="preserve">
@@ -139,14 +125,13 @@
         </r>
       </text>
     </comment>
-    <comment ref="D4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000004000000}">
+    <comment ref="D4" authorId="0">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="9"/>
             <rFont val="宋体"/>
-            <family val="3"/>
             <charset val="134"/>
           </rPr>
           <t>Administrator:</t>
@@ -155,7 +140,6 @@
           <rPr>
             <sz val="9"/>
             <rFont val="宋体"/>
-            <family val="3"/>
             <charset val="134"/>
           </rPr>
           <t xml:space="preserve">
@@ -168,7 +152,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38">
   <si>
     <t>ID</t>
   </si>
@@ -176,15 +160,30 @@
     <t>Name</t>
   </si>
   <si>
+    <t>SSS</t>
+  </si>
+  <si>
+    <t>DDD</t>
+  </si>
+  <si>
     <t>int32</t>
   </si>
   <si>
     <t>SampleID</t>
   </si>
   <si>
+    <t>string</t>
+  </si>
+  <si>
+    <t>Vec2</t>
+  </si>
+  <si>
     <t>MakeIndex:true</t>
   </si>
   <si>
+    <t>Mark:Client</t>
+  </si>
+  <si>
     <t>唯一ID</t>
   </si>
   <si>
@@ -194,9 +193,30 @@
     <t>黑猫警长</t>
   </si>
   <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>X:2 Y:3</t>
+  </si>
+  <si>
     <t>邋遢大王</t>
   </si>
   <si>
+    <t>A1</t>
+  </si>
+  <si>
+    <t>X:2 Y:4</t>
+  </si>
+  <si>
+    <t>A2</t>
+  </si>
+  <si>
+    <t>X:2 Y:5</t>
+  </si>
+  <si>
+    <t>A3</t>
+  </si>
+  <si>
     <t>TableName: "AAA" Package: "table" CSClassHeader: "[System.Serializable]"</t>
   </si>
   <si>
@@ -246,41 +266,19 @@
   </si>
   <si>
     <t>注释</t>
-  </si>
-  <si>
-    <t>SSS</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>string</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>A</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>A1</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>A2</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>A3</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>Mark:Client</t>
-    <phoneticPr fontId="8" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="24">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -292,60 +290,173 @@
       <sz val="10"/>
       <color indexed="8"/>
       <name val="微软雅黑"/>
-      <family val="2"/>
       <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="微软雅黑"/>
-      <family val="2"/>
       <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="微软雅黑"/>
-      <family val="2"/>
       <charset val="134"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
-      <name val="宋体"/>
-      <family val="3"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
       <charset val="134"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
-      <name val="宋体"/>
-      <family val="3"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
       <charset val="134"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="9"/>
-      <name val="宋体"/>
-      <family val="3"/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
       <charset val="134"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <name val="宋体"/>
-      <family val="3"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
       <charset val="134"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -358,8 +469,194 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -382,9 +679,251 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -405,24 +944,68 @@
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="1" builtinId="52"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="2" builtinId="42"/>
+    <cellStyle name="强调文字颜色 4" xfId="3" builtinId="41"/>
+    <cellStyle name="输入" xfId="4" builtinId="20"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="5" builtinId="39"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="6" builtinId="38"/>
+    <cellStyle name="货币" xfId="7" builtinId="4"/>
+    <cellStyle name="强调文字颜色 3" xfId="8" builtinId="37"/>
+    <cellStyle name="百分比" xfId="9" builtinId="5"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="10" builtinId="36"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="11" builtinId="48"/>
+    <cellStyle name="强调文字颜色 2" xfId="12" builtinId="33"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="13" builtinId="32"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="14" builtinId="44"/>
+    <cellStyle name="计算" xfId="15" builtinId="22"/>
+    <cellStyle name="强调文字颜色 1" xfId="16" builtinId="29"/>
+    <cellStyle name="适中" xfId="17" builtinId="28"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="18" builtinId="46"/>
+    <cellStyle name="好" xfId="19" builtinId="26"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="20" builtinId="30"/>
+    <cellStyle name="汇总" xfId="21" builtinId="25"/>
+    <cellStyle name="差" xfId="22" builtinId="27"/>
+    <cellStyle name="检查单元格" xfId="23" builtinId="23"/>
+    <cellStyle name="输出" xfId="24" builtinId="21"/>
+    <cellStyle name="标题 1" xfId="25" builtinId="16"/>
+    <cellStyle name="解释性文本" xfId="26" builtinId="53"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="27" builtinId="34"/>
+    <cellStyle name="标题 4" xfId="28" builtinId="19"/>
+    <cellStyle name="货币[0]" xfId="29" builtinId="7"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="30" builtinId="43"/>
+    <cellStyle name="千位分隔" xfId="31" builtinId="3"/>
+    <cellStyle name="已访问的超链接" xfId="32" builtinId="9"/>
+    <cellStyle name="标题" xfId="33" builtinId="15"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="34" builtinId="35"/>
+    <cellStyle name="警告文本" xfId="35" builtinId="11"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="36" builtinId="40"/>
+    <cellStyle name="注释" xfId="37" builtinId="10"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="38" builtinId="50"/>
+    <cellStyle name="强调文字颜色 5" xfId="39" builtinId="45"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="40" builtinId="51"/>
+    <cellStyle name="超链接" xfId="41" builtinId="8"/>
+    <cellStyle name="千位分隔[0]" xfId="42" builtinId="6"/>
+    <cellStyle name="标题 2" xfId="43" builtinId="17"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
+    <cellStyle name="标题 3" xfId="45" builtinId="18"/>
+    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="47" builtinId="31"/>
+    <cellStyle name="链接单元格" xfId="48" builtinId="24"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
@@ -436,21 +1019,15 @@
       <xdr:row>18</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
+    <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="文本框 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="2" name="文本框 1"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2498090" y="2356485"/>
-          <a:ext cx="0" cy="1011555"/>
+          <a:off x="2566670" y="2356485"/>
+          <a:ext cx="382905" cy="1011555"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -601,21 +1178,15 @@
       <xdr:row>18</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
+    <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="文本框 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1D409B2D-1773-FE4A-8156-BFB8AFF38B9C}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="3" name="文本框 2"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2746375" y="2752725"/>
-          <a:ext cx="657225" cy="1209675"/>
+          <a:off x="4349750" y="2356485"/>
+          <a:ext cx="382905" cy="1011555"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1008,26 +1579,26 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="17"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="7" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="1" width="17.6640625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="17.6634615384615" style="3" customWidth="1"/>
     <col min="2" max="3" width="27" style="3" customWidth="1"/>
     <col min="4" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1035,71 +1606,86 @@
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>26</v>
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:4">
       <c r="A2" s="4" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>27</v>
+        <v>6</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="4" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4" t="s">
-        <v>32</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="2" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:4">
       <c r="A5" s="3">
         <v>1</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>28</v>
+        <v>13</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:4">
       <c r="A6" s="3">
         <v>2</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>29</v>
+        <v>16</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:4">
       <c r="A7" s="3">
         <v>3</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>30</v>
+        <v>18</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -1107,98 +1693,103 @@
         <v>4</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="8" type="noConversion"/>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <drawing r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <headerFooter/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelRow="3" outlineLevelCol="7"/>
   <cols>
     <col min="1" max="1" width="10.5" customWidth="1"/>
-    <col min="2" max="3" width="11.6640625" customWidth="1"/>
-    <col min="4" max="6" width="13.1640625" customWidth="1"/>
-    <col min="7" max="7" width="29.1640625" customWidth="1"/>
-    <col min="8" max="8" width="28.1640625" customWidth="1"/>
+    <col min="2" max="3" width="11.6634615384615" customWidth="1"/>
+    <col min="4" max="6" width="13.1634615384615" customWidth="1"/>
+    <col min="7" max="7" width="29.1634615384615" customWidth="1"/>
+    <col min="8" max="8" width="28.1634615384615" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="D2" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="F2" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="G2" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="H2" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="16">
+    <row r="3" spans="1:8">
       <c r="A3" s="2" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:8"/>
+    <row r="4" spans="4:4">
+      <c r="D4"/>
+    </row>
   </sheetData>
-  <phoneticPr fontId="8" type="noConversion"/>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <legacyDrawing r:id="rId1"/>
+  <headerFooter/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>